<commit_message>
renamed headers in tables
</commit_message>
<xml_diff>
--- a/DataAnalyst_Ecom_data_Report.xlsx
+++ b/DataAnalyst_Ecom_data_Report.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alexandre_1/PycharmProjects/IXIS/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6821BC90-184D-F143-B1D8-8F914C0648AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="17800" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PerMonthPerDevice" sheetId="1" r:id="rId1"/>
     <sheet name="PerDevicePerMonth" sheetId="2" r:id="rId2"/>
     <sheet name="MonthOverMonthComparison" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
   <si>
     <t>sessions</t>
   </si>
@@ -24,13 +30,13 @@
     <t>transactions</t>
   </si>
   <si>
-    <t>QTY</t>
+    <t>quantity</t>
   </si>
   <si>
     <t>ECR</t>
   </si>
   <si>
-    <t>QtyPerTransaction</t>
+    <t>quantity per transaction</t>
   </si>
   <si>
     <t>dim_date</t>
@@ -62,12 +68,18 @@
   <si>
     <t>addsToCart</t>
   </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>Quantity Per Transaction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -130,6 +145,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -176,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,9 +231,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,6 +283,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -417,14 +476,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -450,11 +520,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>2012</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -470,15 +540,15 @@
         <v>18547</v>
       </c>
       <c r="G2">
-        <v>0.0319024294261975</v>
+        <v>3.1902429426197497E-2</v>
       </c>
       <c r="H2">
-        <v>1.733202504438837</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+        <v>1.7332025044388371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -492,15 +562,15 @@
         <v>4557</v>
       </c>
       <c r="G3">
-        <v>0.009386284219309655</v>
+        <v>9.3862842193096555E-3</v>
       </c>
       <c r="H3">
         <v>1.769021739130435</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -514,15 +584,15 @@
         <v>8700</v>
       </c>
       <c r="G4">
-        <v>0.03077175097815609</v>
+        <v>3.0771750978156091E-2</v>
       </c>
       <c r="H4">
         <v>1.781326781326781</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -538,15 +608,15 @@
         <v>23316</v>
       </c>
       <c r="G5">
-        <v>0.03293213867613415</v>
+        <v>3.2932138676134148E-2</v>
       </c>
       <c r="H5">
-        <v>1.805762081784387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+        <v>1.8057620817843869</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
@@ -560,15 +630,15 @@
         <v>5572</v>
       </c>
       <c r="G6">
-        <v>0.01148586857117972</v>
+        <v>1.148586857117972E-2</v>
       </c>
       <c r="H6">
         <v>1.760505529225908</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
@@ -582,15 +652,15 @@
         <v>5760</v>
       </c>
       <c r="G7">
-        <v>0.02067700732283769</v>
+        <v>2.0677007322837691E-2</v>
       </c>
       <c r="H7">
-        <v>1.798875702685821</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1">
+        <v>1.7988757026858211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -606,15 +676,15 @@
         <v>16507</v>
       </c>
       <c r="G8">
-        <v>0.03262076980324154</v>
+        <v>3.2620769803241537E-2</v>
       </c>
       <c r="H8">
-        <v>1.855135985614745</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+        <v>1.8551359856147449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -628,15 +698,15 @@
         <v>4050</v>
       </c>
       <c r="G9">
-        <v>0.01078893827966052</v>
+        <v>1.078893827966052E-2</v>
       </c>
       <c r="H9">
-        <v>1.700965980680386</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+        <v>1.7009659806803861</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
@@ -650,15 +720,15 @@
         <v>7869</v>
       </c>
       <c r="G10">
-        <v>0.02588168541251707</v>
+        <v>2.5881685412517071E-2</v>
       </c>
       <c r="H10">
-        <v>1.796985613153688</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1">
+        <v>1.7969856131536881</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -674,15 +744,15 @@
         <v>17675</v>
       </c>
       <c r="G11">
-        <v>0.03096649288692423</v>
+        <v>3.096649288692423E-2</v>
       </c>
       <c r="H11">
-        <v>1.885735623599701</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+        <v>1.8857356235997009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
@@ -696,15 +766,15 @@
         <v>4446</v>
       </c>
       <c r="G12">
-        <v>0.01012355086267893</v>
+        <v>1.012355086267893E-2</v>
       </c>
       <c r="H12">
         <v>1.838709677419355</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
@@ -718,15 +788,15 @@
         <v>4505</v>
       </c>
       <c r="G13">
-        <v>0.02319154498263435</v>
+        <v>2.319154498263435E-2</v>
       </c>
       <c r="H13">
-        <v>1.813607085346216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1">
+        <v>1.8136070853462161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -742,15 +812,15 @@
         <v>18778</v>
       </c>
       <c r="G14">
-        <v>0.03227144180071527</v>
+        <v>3.227144180071527E-2</v>
       </c>
       <c r="H14">
         <v>1.814299516908213</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
@@ -764,15 +834,15 @@
         <v>3407</v>
       </c>
       <c r="G15">
-        <v>0.01115037913525846</v>
+        <v>1.1150379135258459E-2</v>
       </c>
       <c r="H15">
-        <v>1.708625877632899</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+        <v>1.7086258776328991</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
@@ -786,15 +856,15 @@
         <v>5947</v>
       </c>
       <c r="G16">
-        <v>0.02302600643831157</v>
+        <v>2.3026006438311569E-2</v>
       </c>
       <c r="H16">
         <v>1.868363179390512</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2">
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -810,15 +880,15 @@
         <v>19947</v>
       </c>
       <c r="G17">
-        <v>0.03749539904041741</v>
+        <v>3.7495399040417411E-2</v>
       </c>
       <c r="H17">
-        <v>1.71764401963317</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+        <v>1.7176440196331699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
@@ -832,15 +902,15 @@
         <v>5672</v>
       </c>
       <c r="G18">
-        <v>0.01346804218678699</v>
+        <v>1.346804218678699E-2</v>
       </c>
       <c r="H18">
-        <v>1.796073464217859</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+        <v>1.7960734642178591</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
@@ -854,17 +924,17 @@
         <v>9133</v>
       </c>
       <c r="G19">
-        <v>0.02101574755026789</v>
+        <v>2.1015747550267892E-2</v>
       </c>
       <c r="H19">
         <v>1.770647537805351</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>2013</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -880,15 +950,15 @@
         <v>25424</v>
       </c>
       <c r="G20">
-        <v>0.03503224348082281</v>
+        <v>3.503224348082281E-2</v>
       </c>
       <c r="H20">
-        <v>1.843253824403683</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+        <v>1.8432538244036829</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
@@ -902,15 +972,15 @@
         <v>7257</v>
       </c>
       <c r="G21">
-        <v>0.01276092581102123</v>
+        <v>1.276092581102123E-2</v>
       </c>
       <c r="H21">
         <v>1.664449541284404</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
@@ -924,15 +994,15 @@
         <v>6165</v>
       </c>
       <c r="G22">
-        <v>0.0206985376759558</v>
+        <v>2.0698537675955801E-2</v>
       </c>
       <c r="H22">
         <v>1.809509832697388</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2">
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -948,15 +1018,15 @@
         <v>18437</v>
       </c>
       <c r="G23">
-        <v>0.03916698972669122</v>
+        <v>3.916698972669122E-2</v>
       </c>
       <c r="H23">
-        <v>1.900917620373234</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+        <v>1.9009176203732341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
@@ -970,15 +1040,15 @@
         <v>3915</v>
       </c>
       <c r="G24">
-        <v>0.01062073068165501</v>
+        <v>1.062073068165501E-2</v>
       </c>
       <c r="H24">
-        <v>1.890391115403187</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+        <v>1.8903911154031869</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
@@ -992,15 +1062,15 @@
         <v>4696</v>
       </c>
       <c r="G25">
-        <v>0.02226786494298274</v>
+        <v>2.2267864942982739E-2</v>
       </c>
       <c r="H25">
         <v>1.959933222036728</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2">
         <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1016,15 +1086,15 @@
         <v>17362</v>
       </c>
       <c r="G26">
-        <v>0.03362667065040283</v>
+        <v>3.3626670650402833E-2</v>
       </c>
       <c r="H26">
-        <v>1.793780349209629</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+        <v>1.7937803492096289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1038,15 +1108,15 @@
         <v>6455</v>
       </c>
       <c r="G27">
-        <v>0.01195412555112324</v>
+        <v>1.195412555112324E-2</v>
       </c>
       <c r="H27">
-        <v>1.771405049396268</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+        <v>1.7714050493962681</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
@@ -1060,15 +1130,15 @@
         <v>8265</v>
       </c>
       <c r="G28">
-        <v>0.02284464519681266</v>
+        <v>2.284464519681266E-2</v>
       </c>
       <c r="H28">
         <v>1.844454362865432</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2">
         <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1084,15 +1154,15 @@
         <v>34200</v>
       </c>
       <c r="G29">
-        <v>0.03324699124244507</v>
+        <v>3.3246991242445068E-2</v>
       </c>
       <c r="H29">
         <v>1.812592749629002</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
@@ -1106,15 +1176,15 @@
         <v>7752</v>
       </c>
       <c r="G30">
-        <v>0.009956637448123128</v>
+        <v>9.956637448123128E-3</v>
       </c>
       <c r="H30">
         <v>1.811214953271028</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
@@ -1128,15 +1198,15 @@
         <v>12994</v>
       </c>
       <c r="G31">
-        <v>0.0241312128432457</v>
+        <v>2.4131212843245702E-2</v>
       </c>
       <c r="H31">
-        <v>1.799473757097355</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1">
+        <v>1.7994737570973549</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2">
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1152,15 +1222,15 @@
         <v>33208</v>
       </c>
       <c r="G32">
-        <v>0.0345334675963749</v>
+        <v>3.4533467596374899E-2</v>
       </c>
       <c r="H32">
         <v>1.827024647887324</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
@@ -1174,15 +1244,15 @@
         <v>9790</v>
       </c>
       <c r="G33">
-        <v>0.01320901131294595</v>
+        <v>1.320901131294595E-2</v>
       </c>
       <c r="H33">
-        <v>1.808608904489193</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+        <v>1.8086089044891931</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1196,15 +1266,15 @@
         <v>8631</v>
       </c>
       <c r="G34">
-        <v>0.02100536949757782</v>
+        <v>2.1005369497577819E-2</v>
       </c>
       <c r="H34">
         <v>1.798125</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2">
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1220,15 +1290,15 @@
         <v>35146</v>
       </c>
       <c r="G35">
-        <v>0.03490467437921217</v>
+        <v>3.4904674379212172E-2</v>
       </c>
       <c r="H35">
-        <v>1.814455343314404</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+        <v>1.8144553433144039</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
@@ -1242,15 +1312,15 @@
         <v>13017</v>
       </c>
       <c r="G36">
-        <v>0.01407838079626805</v>
+        <v>1.4078380796268049E-2</v>
       </c>
       <c r="H36">
-        <v>1.756206152185645</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+        <v>1.7562061521856449</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="1" t="s">
         <v>9</v>
       </c>
@@ -1264,10 +1334,10 @@
         <v>13728</v>
       </c>
       <c r="G37">
-        <v>0.02522990244394349</v>
+        <v>2.5229902443943492E-2</v>
       </c>
       <c r="H37">
-        <v>1.769984528107272</v>
+        <v>1.7699845281072719</v>
       </c>
     </row>
   </sheetData>
@@ -1292,14 +1362,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1325,11 +1406,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>2012</v>
       </c>
       <c r="C2" s="1">
@@ -1345,15 +1426,15 @@
         <v>18547</v>
       </c>
       <c r="G2">
-        <v>0.0319024294261975</v>
+        <v>3.1902429426197497E-2</v>
       </c>
       <c r="H2">
-        <v>1.733202504438837</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+        <v>1.7332025044388371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="1">
         <v>8</v>
       </c>
@@ -1367,15 +1448,15 @@
         <v>23316</v>
       </c>
       <c r="G3">
-        <v>0.03293213867613415</v>
+        <v>3.2932138676134148E-2</v>
       </c>
       <c r="H3">
-        <v>1.805762081784387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+        <v>1.8057620817843869</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1">
         <v>9</v>
       </c>
@@ -1389,15 +1470,15 @@
         <v>16507</v>
       </c>
       <c r="G4">
-        <v>0.03262076980324154</v>
+        <v>3.2620769803241537E-2</v>
       </c>
       <c r="H4">
-        <v>1.855135985614745</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+        <v>1.8551359856147449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="1">
         <v>10</v>
       </c>
@@ -1411,15 +1492,15 @@
         <v>17675</v>
       </c>
       <c r="G5">
-        <v>0.03096649288692423</v>
+        <v>3.096649288692423E-2</v>
       </c>
       <c r="H5">
-        <v>1.885735623599701</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+        <v>1.8857356235997009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1">
         <v>11</v>
       </c>
@@ -1433,15 +1514,15 @@
         <v>18778</v>
       </c>
       <c r="G6">
-        <v>0.03227144180071527</v>
+        <v>3.227144180071527E-2</v>
       </c>
       <c r="H6">
         <v>1.814299516908213</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1">
         <v>12</v>
       </c>
@@ -1455,15 +1536,15 @@
         <v>19947</v>
       </c>
       <c r="G7">
-        <v>0.03749539904041741</v>
+        <v>3.7495399040417411E-2</v>
       </c>
       <c r="H7">
-        <v>1.71764401963317</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1">
+        <v>1.7176440196331699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
         <v>2013</v>
       </c>
       <c r="C8" s="1">
@@ -1479,15 +1560,15 @@
         <v>25424</v>
       </c>
       <c r="G8">
-        <v>0.03503224348082281</v>
+        <v>3.503224348082281E-2</v>
       </c>
       <c r="H8">
-        <v>1.843253824403683</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+        <v>1.8432538244036829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="1">
         <v>2</v>
       </c>
@@ -1501,15 +1582,15 @@
         <v>18437</v>
       </c>
       <c r="G9">
-        <v>0.03916698972669122</v>
+        <v>3.916698972669122E-2</v>
       </c>
       <c r="H9">
-        <v>1.900917620373234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+        <v>1.9009176203732341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1">
         <v>3</v>
       </c>
@@ -1523,15 +1604,15 @@
         <v>17362</v>
       </c>
       <c r="G10">
-        <v>0.03362667065040283</v>
+        <v>3.3626670650402833E-2</v>
       </c>
       <c r="H10">
-        <v>1.793780349209629</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+        <v>1.7937803492096289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="1">
         <v>4</v>
       </c>
@@ -1545,15 +1626,15 @@
         <v>34200</v>
       </c>
       <c r="G11">
-        <v>0.03324699124244507</v>
+        <v>3.3246991242445068E-2</v>
       </c>
       <c r="H11">
         <v>1.812592749629002</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1">
         <v>5</v>
       </c>
@@ -1567,15 +1648,15 @@
         <v>33208</v>
       </c>
       <c r="G12">
-        <v>0.0345334675963749</v>
+        <v>3.4533467596374899E-2</v>
       </c>
       <c r="H12">
         <v>1.827024647887324</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -1589,17 +1670,17 @@
         <v>35146</v>
       </c>
       <c r="G13">
-        <v>0.03490467437921217</v>
+        <v>3.4904674379212172E-2</v>
       </c>
       <c r="H13">
-        <v>1.814455343314404</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1" t="s">
+        <v>1.8144553433144039</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>2012</v>
       </c>
       <c r="C14" s="1">
@@ -1615,15 +1696,15 @@
         <v>4557</v>
       </c>
       <c r="G14">
-        <v>0.009386284219309655</v>
+        <v>9.3862842193096555E-3</v>
       </c>
       <c r="H14">
         <v>1.769021739130435</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1">
         <v>8</v>
       </c>
@@ -1637,15 +1718,15 @@
         <v>5572</v>
       </c>
       <c r="G15">
-        <v>0.01148586857117972</v>
+        <v>1.148586857117972E-2</v>
       </c>
       <c r="H15">
         <v>1.760505529225908</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1">
         <v>9</v>
       </c>
@@ -1659,15 +1740,15 @@
         <v>4050</v>
       </c>
       <c r="G16">
-        <v>0.01078893827966052</v>
+        <v>1.078893827966052E-2</v>
       </c>
       <c r="H16">
-        <v>1.700965980680386</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+        <v>1.7009659806803861</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="1">
         <v>10</v>
       </c>
@@ -1681,15 +1762,15 @@
         <v>4446</v>
       </c>
       <c r="G17">
-        <v>0.01012355086267893</v>
+        <v>1.012355086267893E-2</v>
       </c>
       <c r="H17">
         <v>1.838709677419355</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="1">
         <v>11</v>
       </c>
@@ -1703,15 +1784,15 @@
         <v>3407</v>
       </c>
       <c r="G18">
-        <v>0.01115037913525846</v>
+        <v>1.1150379135258459E-2</v>
       </c>
       <c r="H18">
-        <v>1.708625877632899</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+        <v>1.7086258776328991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1">
         <v>12</v>
       </c>
@@ -1725,15 +1806,15 @@
         <v>5672</v>
       </c>
       <c r="G19">
-        <v>0.01346804218678699</v>
+        <v>1.346804218678699E-2</v>
       </c>
       <c r="H19">
-        <v>1.796073464217859</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1">
+        <v>1.7960734642178591</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2">
         <v>2013</v>
       </c>
       <c r="C20" s="1">
@@ -1749,15 +1830,15 @@
         <v>7257</v>
       </c>
       <c r="G20">
-        <v>0.01276092581102123</v>
+        <v>1.276092581102123E-2</v>
       </c>
       <c r="H20">
         <v>1.664449541284404</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1">
         <v>2</v>
       </c>
@@ -1771,15 +1852,15 @@
         <v>3915</v>
       </c>
       <c r="G21">
-        <v>0.01062073068165501</v>
+        <v>1.062073068165501E-2</v>
       </c>
       <c r="H21">
-        <v>1.890391115403187</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+        <v>1.8903911154031869</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="1">
         <v>3</v>
       </c>
@@ -1793,15 +1874,15 @@
         <v>6455</v>
       </c>
       <c r="G22">
-        <v>0.01195412555112324</v>
+        <v>1.195412555112324E-2</v>
       </c>
       <c r="H22">
-        <v>1.771405049396268</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+        <v>1.7714050493962681</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="1">
         <v>4</v>
       </c>
@@ -1815,15 +1896,15 @@
         <v>7752</v>
       </c>
       <c r="G23">
-        <v>0.009956637448123128</v>
+        <v>9.956637448123128E-3</v>
       </c>
       <c r="H23">
         <v>1.811214953271028</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="1">
         <v>5</v>
       </c>
@@ -1837,15 +1918,15 @@
         <v>9790</v>
       </c>
       <c r="G24">
-        <v>0.01320901131294595</v>
+        <v>1.320901131294595E-2</v>
       </c>
       <c r="H24">
-        <v>1.808608904489193</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+        <v>1.8086089044891931</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="1">
         <v>6</v>
       </c>
@@ -1859,17 +1940,17 @@
         <v>13017</v>
       </c>
       <c r="G25">
-        <v>0.01407838079626805</v>
+        <v>1.4078380796268049E-2</v>
       </c>
       <c r="H25">
-        <v>1.756206152185645</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1" t="s">
+        <v>1.7562061521856449</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>2012</v>
       </c>
       <c r="C26" s="1">
@@ -1885,15 +1966,15 @@
         <v>8700</v>
       </c>
       <c r="G26">
-        <v>0.03077175097815609</v>
+        <v>3.0771750978156091E-2</v>
       </c>
       <c r="H26">
         <v>1.781326781326781</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="1">
         <v>8</v>
       </c>
@@ -1907,15 +1988,15 @@
         <v>5760</v>
       </c>
       <c r="G27">
-        <v>0.02067700732283769</v>
+        <v>2.0677007322837691E-2</v>
       </c>
       <c r="H27">
-        <v>1.798875702685821</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+        <v>1.7988757026858211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="1">
         <v>9</v>
       </c>
@@ -1929,15 +2010,15 @@
         <v>7869</v>
       </c>
       <c r="G28">
-        <v>0.02588168541251707</v>
+        <v>2.5881685412517071E-2</v>
       </c>
       <c r="H28">
-        <v>1.796985613153688</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+        <v>1.7969856131536881</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
       <c r="C29" s="1">
         <v>10</v>
       </c>
@@ -1951,15 +2032,15 @@
         <v>4505</v>
       </c>
       <c r="G29">
-        <v>0.02319154498263435</v>
+        <v>2.319154498263435E-2</v>
       </c>
       <c r="H29">
-        <v>1.813607085346216</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+        <v>1.8136070853462161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="1">
         <v>11</v>
       </c>
@@ -1973,15 +2054,15 @@
         <v>5947</v>
       </c>
       <c r="G30">
-        <v>0.02302600643831157</v>
+        <v>2.3026006438311569E-2</v>
       </c>
       <c r="H30">
         <v>1.868363179390512</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="1">
         <v>12</v>
       </c>
@@ -1995,15 +2076,15 @@
         <v>9133</v>
       </c>
       <c r="G31">
-        <v>0.02101574755026789</v>
+        <v>2.1015747550267892E-2</v>
       </c>
       <c r="H31">
         <v>1.770647537805351</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2">
         <v>2013</v>
       </c>
       <c r="C32" s="1">
@@ -2019,15 +2100,15 @@
         <v>6165</v>
       </c>
       <c r="G32">
-        <v>0.0206985376759558</v>
+        <v>2.0698537675955801E-2</v>
       </c>
       <c r="H32">
         <v>1.809509832697388</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="1">
         <v>2</v>
       </c>
@@ -2041,15 +2122,15 @@
         <v>4696</v>
       </c>
       <c r="G33">
-        <v>0.02226786494298274</v>
+        <v>2.2267864942982739E-2</v>
       </c>
       <c r="H33">
         <v>1.959933222036728</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="1">
         <v>3</v>
       </c>
@@ -2063,15 +2144,15 @@
         <v>8265</v>
       </c>
       <c r="G34">
-        <v>0.02284464519681266</v>
+        <v>2.284464519681266E-2</v>
       </c>
       <c r="H34">
         <v>1.844454362865432</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="1">
         <v>4</v>
       </c>
@@ -2085,15 +2166,15 @@
         <v>12994</v>
       </c>
       <c r="G35">
-        <v>0.0241312128432457</v>
+        <v>2.4131212843245702E-2</v>
       </c>
       <c r="H35">
-        <v>1.799473757097355</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+        <v>1.7994737570973549</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="1">
         <v>5</v>
       </c>
@@ -2107,15 +2188,15 @@
         <v>8631</v>
       </c>
       <c r="G36">
-        <v>0.02100536949757782</v>
+        <v>2.1005369497577819E-2</v>
       </c>
       <c r="H36">
         <v>1.798125</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="1">
         <v>6</v>
       </c>
@@ -2129,10 +2210,10 @@
         <v>13728</v>
       </c>
       <c r="G37">
-        <v>0.02522990244394349</v>
+        <v>2.5229902443943492E-2</v>
       </c>
       <c r="H37">
-        <v>1.769984528107272</v>
+        <v>1.7699845281072719</v>
       </c>
     </row>
   </sheetData>
@@ -2152,14 +2233,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <v>10</v>
       </c>
@@ -2173,7 +2254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -2184,7 +2265,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2195,7 +2276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -2209,10 +2290,10 @@
         <v>-28750</v>
       </c>
       <c r="E4">
-        <v>-0.2102837916910474</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>-0.21028379169104741</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2226,10 +2307,10 @@
         <v>224195</v>
       </c>
       <c r="E5">
-        <v>0.1925017108305664</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.19250171083056641</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2243,12 +2324,12 @@
         <v>6149</v>
       </c>
       <c r="E6">
-        <v>0.2165979780901053</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0.21659797809010531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>51629</v>
@@ -2260,29 +2341,29 @@
         <v>10262</v>
       </c>
       <c r="E7">
-        <v>0.1987642603962889</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.19876426039628889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8">
-        <v>0.0243757937008807</v>
+        <v>2.43757937008807E-2</v>
       </c>
       <c r="C8">
-        <v>0.02486834279690733</v>
+        <v>2.486834279690733E-2</v>
       </c>
       <c r="D8">
-        <v>0.0004925490960266329</v>
+        <v>4.9254909602663294E-4</v>
       </c>
       <c r="E8">
-        <v>0.02020648443578012</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>2.0206484435780121E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>1.818626932966994</v>
@@ -2291,10 +2372,10 @@
         <v>1.791968266836528</v>
       </c>
       <c r="D9">
-        <v>-0.02665866613046619</v>
+        <v>-2.6658666130466191E-2</v>
       </c>
       <c r="E9">
-        <v>-0.01465867773495138</v>
+        <v>-1.4658677734951379E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed headers to make tables easier to read
</commit_message>
<xml_diff>
--- a/DataAnalyst_Ecom_data_Report.xlsx
+++ b/DataAnalyst_Ecom_data_Report.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alexandre_1/PycharmProjects/IXIS/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6821BC90-184D-F143-B1D8-8F914C0648AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="17800" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="PerMonthPerDevice" sheetId="1" r:id="rId1"/>
     <sheet name="PerDevicePerMonth" sheetId="2" r:id="rId2"/>
     <sheet name="MonthOverMonthComparison" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
   <si>
     <t>sessions</t>
   </si>
@@ -54,10 +48,16 @@
     <t>tablet</t>
   </si>
   <si>
-    <t>abs_diff</t>
+    <t>prior month</t>
   </si>
   <si>
-    <t>rel_diff</t>
+    <t>last month</t>
+  </si>
+  <si>
+    <t>absolute difference</t>
+  </si>
+  <si>
+    <t>relative difference</t>
   </si>
   <si>
     <t>dim_year</t>
@@ -78,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,11 +131,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -145,14 +142,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -199,7 +188,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,27 +220,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,24 +254,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -476,25 +429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -520,11 +462,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
         <v>2012</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -540,15 +482,15 @@
         <v>18547</v>
       </c>
       <c r="G2">
-        <v>3.1902429426197497E-2</v>
+        <v>0.0319024294261975</v>
       </c>
       <c r="H2">
-        <v>1.7332025044388371</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+        <v>1.733202504438837</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -562,15 +504,15 @@
         <v>4557</v>
       </c>
       <c r="G3">
-        <v>9.3862842193096555E-3</v>
+        <v>0.009386284219309655</v>
       </c>
       <c r="H3">
         <v>1.769021739130435</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -584,15 +526,15 @@
         <v>8700</v>
       </c>
       <c r="G4">
-        <v>3.0771750978156091E-2</v>
+        <v>0.03077175097815609</v>
       </c>
       <c r="H4">
         <v>1.781326781326781</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2">
+    <row r="5" spans="1:8">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -608,15 +550,15 @@
         <v>23316</v>
       </c>
       <c r="G5">
-        <v>3.2932138676134148E-2</v>
+        <v>0.03293213867613415</v>
       </c>
       <c r="H5">
-        <v>1.8057620817843869</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+        <v>1.805762081784387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
@@ -630,15 +572,15 @@
         <v>5572</v>
       </c>
       <c r="G6">
-        <v>1.148586857117972E-2</v>
+        <v>0.01148586857117972</v>
       </c>
       <c r="H6">
         <v>1.760505529225908</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
@@ -652,15 +594,15 @@
         <v>5760</v>
       </c>
       <c r="G7">
-        <v>2.0677007322837691E-2</v>
+        <v>0.02067700732283769</v>
       </c>
       <c r="H7">
-        <v>1.7988757026858211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2">
+        <v>1.798875702685821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -676,15 +618,15 @@
         <v>16507</v>
       </c>
       <c r="G8">
-        <v>3.2620769803241537E-2</v>
+        <v>0.03262076980324154</v>
       </c>
       <c r="H8">
-        <v>1.8551359856147449</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+        <v>1.855135985614745</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -698,15 +640,15 @@
         <v>4050</v>
       </c>
       <c r="G9">
-        <v>1.078893827966052E-2</v>
+        <v>0.01078893827966052</v>
       </c>
       <c r="H9">
-        <v>1.7009659806803861</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+        <v>1.700965980680386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
@@ -720,15 +662,15 @@
         <v>7869</v>
       </c>
       <c r="G10">
-        <v>2.5881685412517071E-2</v>
+        <v>0.02588168541251707</v>
       </c>
       <c r="H10">
-        <v>1.7969856131536881</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2">
+        <v>1.796985613153688</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -744,15 +686,15 @@
         <v>17675</v>
       </c>
       <c r="G11">
-        <v>3.096649288692423E-2</v>
+        <v>0.03096649288692423</v>
       </c>
       <c r="H11">
-        <v>1.8857356235997009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+        <v>1.885735623599701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
@@ -766,15 +708,15 @@
         <v>4446</v>
       </c>
       <c r="G12">
-        <v>1.012355086267893E-2</v>
+        <v>0.01012355086267893</v>
       </c>
       <c r="H12">
         <v>1.838709677419355</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
@@ -788,15 +730,15 @@
         <v>4505</v>
       </c>
       <c r="G13">
-        <v>2.319154498263435E-2</v>
+        <v>0.02319154498263435</v>
       </c>
       <c r="H13">
-        <v>1.8136070853462161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2">
+        <v>1.813607085346216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -812,15 +754,15 @@
         <v>18778</v>
       </c>
       <c r="G14">
-        <v>3.227144180071527E-2</v>
+        <v>0.03227144180071527</v>
       </c>
       <c r="H14">
         <v>1.814299516908213</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
@@ -834,15 +776,15 @@
         <v>3407</v>
       </c>
       <c r="G15">
-        <v>1.1150379135258459E-2</v>
+        <v>0.01115037913525846</v>
       </c>
       <c r="H15">
-        <v>1.7086258776328991</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+        <v>1.708625877632899</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
@@ -856,15 +798,15 @@
         <v>5947</v>
       </c>
       <c r="G16">
-        <v>2.3026006438311569E-2</v>
+        <v>0.02302600643831157</v>
       </c>
       <c r="H16">
         <v>1.868363179390512</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2">
+    <row r="17" spans="1:8">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1">
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -880,15 +822,15 @@
         <v>19947</v>
       </c>
       <c r="G17">
-        <v>3.7495399040417411E-2</v>
+        <v>0.03749539904041741</v>
       </c>
       <c r="H17">
-        <v>1.7176440196331699</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+        <v>1.71764401963317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
@@ -902,15 +844,15 @@
         <v>5672</v>
       </c>
       <c r="G18">
-        <v>1.346804218678699E-2</v>
+        <v>0.01346804218678699</v>
       </c>
       <c r="H18">
-        <v>1.7960734642178591</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+        <v>1.796073464217859</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
@@ -924,17 +866,17 @@
         <v>9133</v>
       </c>
       <c r="G19">
-        <v>2.1015747550267892E-2</v>
+        <v>0.02101574755026789</v>
       </c>
       <c r="H19">
         <v>1.770647537805351</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
         <v>2013</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -950,15 +892,15 @@
         <v>25424</v>
       </c>
       <c r="G20">
-        <v>3.503224348082281E-2</v>
+        <v>0.03503224348082281</v>
       </c>
       <c r="H20">
-        <v>1.8432538244036829</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+        <v>1.843253824403683</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
@@ -972,15 +914,15 @@
         <v>7257</v>
       </c>
       <c r="G21">
-        <v>1.276092581102123E-2</v>
+        <v>0.01276092581102123</v>
       </c>
       <c r="H21">
         <v>1.664449541284404</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
@@ -994,15 +936,15 @@
         <v>6165</v>
       </c>
       <c r="G22">
-        <v>2.0698537675955801E-2</v>
+        <v>0.0206985376759558</v>
       </c>
       <c r="H22">
         <v>1.809509832697388</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2">
+    <row r="23" spans="1:8">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1018,15 +960,15 @@
         <v>18437</v>
       </c>
       <c r="G23">
-        <v>3.916698972669122E-2</v>
+        <v>0.03916698972669122</v>
       </c>
       <c r="H23">
-        <v>1.9009176203732341</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+        <v>1.900917620373234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1040,15 +982,15 @@
         <v>3915</v>
       </c>
       <c r="G24">
-        <v>1.062073068165501E-2</v>
+        <v>0.01062073068165501</v>
       </c>
       <c r="H24">
-        <v>1.8903911154031869</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+        <v>1.890391115403187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1062,15 +1004,15 @@
         <v>4696</v>
       </c>
       <c r="G25">
-        <v>2.2267864942982739E-2</v>
+        <v>0.02226786494298274</v>
       </c>
       <c r="H25">
         <v>1.959933222036728</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2">
+    <row r="26" spans="1:8">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1">
         <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1086,15 +1028,15 @@
         <v>17362</v>
       </c>
       <c r="G26">
-        <v>3.3626670650402833E-2</v>
+        <v>0.03362667065040283</v>
       </c>
       <c r="H26">
-        <v>1.7937803492096289</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+        <v>1.793780349209629</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1108,15 +1050,15 @@
         <v>6455</v>
       </c>
       <c r="G27">
-        <v>1.195412555112324E-2</v>
+        <v>0.01195412555112324</v>
       </c>
       <c r="H27">
-        <v>1.7714050493962681</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+        <v>1.771405049396268</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
@@ -1130,15 +1072,15 @@
         <v>8265</v>
       </c>
       <c r="G28">
-        <v>2.284464519681266E-2</v>
+        <v>0.02284464519681266</v>
       </c>
       <c r="H28">
         <v>1.844454362865432</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2">
+    <row r="29" spans="1:8">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1">
         <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1154,15 +1096,15 @@
         <v>34200</v>
       </c>
       <c r="G29">
-        <v>3.3246991242445068E-2</v>
+        <v>0.03324699124244507</v>
       </c>
       <c r="H29">
         <v>1.812592749629002</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
@@ -1176,15 +1118,15 @@
         <v>7752</v>
       </c>
       <c r="G30">
-        <v>9.956637448123128E-3</v>
+        <v>0.009956637448123128</v>
       </c>
       <c r="H30">
         <v>1.811214953271028</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
@@ -1198,15 +1140,15 @@
         <v>12994</v>
       </c>
       <c r="G31">
-        <v>2.4131212843245702E-2</v>
+        <v>0.0241312128432457</v>
       </c>
       <c r="H31">
-        <v>1.7994737570973549</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2">
+        <v>1.799473757097355</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1">
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1222,15 +1164,15 @@
         <v>33208</v>
       </c>
       <c r="G32">
-        <v>3.4533467596374899E-2</v>
+        <v>0.0345334675963749</v>
       </c>
       <c r="H32">
         <v>1.827024647887324</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
@@ -1244,15 +1186,15 @@
         <v>9790</v>
       </c>
       <c r="G33">
-        <v>1.320901131294595E-2</v>
+        <v>0.01320901131294595</v>
       </c>
       <c r="H33">
-        <v>1.8086089044891931</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+        <v>1.808608904489193</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1266,15 +1208,15 @@
         <v>8631</v>
       </c>
       <c r="G34">
-        <v>2.1005369497577819E-2</v>
+        <v>0.02100536949757782</v>
       </c>
       <c r="H34">
         <v>1.798125</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2">
+    <row r="35" spans="1:8">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1">
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1290,15 +1232,15 @@
         <v>35146</v>
       </c>
       <c r="G35">
-        <v>3.4904674379212172E-2</v>
+        <v>0.03490467437921217</v>
       </c>
       <c r="H35">
-        <v>1.8144553433144039</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+        <v>1.814455343314404</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
@@ -1312,15 +1254,15 @@
         <v>13017</v>
       </c>
       <c r="G36">
-        <v>1.4078380796268049E-2</v>
+        <v>0.01407838079626805</v>
       </c>
       <c r="H36">
-        <v>1.7562061521856449</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+        <v>1.756206152185645</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>9</v>
       </c>
@@ -1334,10 +1276,10 @@
         <v>13728</v>
       </c>
       <c r="G37">
-        <v>2.5229902443943492E-2</v>
+        <v>0.02522990244394349</v>
       </c>
       <c r="H37">
-        <v>1.7699845281072719</v>
+        <v>1.769984528107272</v>
       </c>
     </row>
   </sheetData>
@@ -1362,25 +1304,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1406,11 +1337,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>2012</v>
       </c>
       <c r="C2" s="1">
@@ -1426,15 +1357,15 @@
         <v>18547</v>
       </c>
       <c r="G2">
-        <v>3.1902429426197497E-2</v>
+        <v>0.0319024294261975</v>
       </c>
       <c r="H2">
-        <v>1.7332025044388371</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+        <v>1.733202504438837</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1">
         <v>8</v>
       </c>
@@ -1448,15 +1379,15 @@
         <v>23316</v>
       </c>
       <c r="G3">
-        <v>3.2932138676134148E-2</v>
+        <v>0.03293213867613415</v>
       </c>
       <c r="H3">
-        <v>1.8057620817843869</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+        <v>1.805762081784387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1">
         <v>9</v>
       </c>
@@ -1470,15 +1401,15 @@
         <v>16507</v>
       </c>
       <c r="G4">
-        <v>3.2620769803241537E-2</v>
+        <v>0.03262076980324154</v>
       </c>
       <c r="H4">
-        <v>1.8551359856147449</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+        <v>1.855135985614745</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="1">
         <v>10</v>
       </c>
@@ -1492,15 +1423,15 @@
         <v>17675</v>
       </c>
       <c r="G5">
-        <v>3.096649288692423E-2</v>
+        <v>0.03096649288692423</v>
       </c>
       <c r="H5">
-        <v>1.8857356235997009</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+        <v>1.885735623599701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1">
         <v>11</v>
       </c>
@@ -1514,15 +1445,15 @@
         <v>18778</v>
       </c>
       <c r="G6">
-        <v>3.227144180071527E-2</v>
+        <v>0.03227144180071527</v>
       </c>
       <c r="H6">
         <v>1.814299516908213</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1">
         <v>12</v>
       </c>
@@ -1536,15 +1467,15 @@
         <v>19947</v>
       </c>
       <c r="G7">
-        <v>3.7495399040417411E-2</v>
+        <v>0.03749539904041741</v>
       </c>
       <c r="H7">
-        <v>1.7176440196331699</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2">
+        <v>1.71764401963317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1">
         <v>2013</v>
       </c>
       <c r="C8" s="1">
@@ -1560,15 +1491,15 @@
         <v>25424</v>
       </c>
       <c r="G8">
-        <v>3.503224348082281E-2</v>
+        <v>0.03503224348082281</v>
       </c>
       <c r="H8">
-        <v>1.8432538244036829</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+        <v>1.843253824403683</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1">
         <v>2</v>
       </c>
@@ -1582,15 +1513,15 @@
         <v>18437</v>
       </c>
       <c r="G9">
-        <v>3.916698972669122E-2</v>
+        <v>0.03916698972669122</v>
       </c>
       <c r="H9">
-        <v>1.9009176203732341</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+        <v>1.900917620373234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1">
         <v>3</v>
       </c>
@@ -1604,15 +1535,15 @@
         <v>17362</v>
       </c>
       <c r="G10">
-        <v>3.3626670650402833E-2</v>
+        <v>0.03362667065040283</v>
       </c>
       <c r="H10">
-        <v>1.7937803492096289</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+        <v>1.793780349209629</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
       <c r="C11" s="1">
         <v>4</v>
       </c>
@@ -1626,15 +1557,15 @@
         <v>34200</v>
       </c>
       <c r="G11">
-        <v>3.3246991242445068E-2</v>
+        <v>0.03324699124244507</v>
       </c>
       <c r="H11">
         <v>1.812592749629002</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="1">
         <v>5</v>
       </c>
@@ -1648,15 +1579,15 @@
         <v>33208</v>
       </c>
       <c r="G12">
-        <v>3.4533467596374899E-2</v>
+        <v>0.0345334675963749</v>
       </c>
       <c r="H12">
         <v>1.827024647887324</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -1670,17 +1601,17 @@
         <v>35146</v>
       </c>
       <c r="G13">
-        <v>3.4904674379212172E-2</v>
+        <v>0.03490467437921217</v>
       </c>
       <c r="H13">
-        <v>1.8144553433144039</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+        <v>1.814455343314404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>2012</v>
       </c>
       <c r="C14" s="1">
@@ -1696,15 +1627,15 @@
         <v>4557</v>
       </c>
       <c r="G14">
-        <v>9.3862842193096555E-3</v>
+        <v>0.009386284219309655</v>
       </c>
       <c r="H14">
         <v>1.769021739130435</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="1">
         <v>8</v>
       </c>
@@ -1718,15 +1649,15 @@
         <v>5572</v>
       </c>
       <c r="G15">
-        <v>1.148586857117972E-2</v>
+        <v>0.01148586857117972</v>
       </c>
       <c r="H15">
         <v>1.760505529225908</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1">
         <v>9</v>
       </c>
@@ -1740,15 +1671,15 @@
         <v>4050</v>
       </c>
       <c r="G16">
-        <v>1.078893827966052E-2</v>
+        <v>0.01078893827966052</v>
       </c>
       <c r="H16">
-        <v>1.7009659806803861</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+        <v>1.700965980680386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="1">
         <v>10</v>
       </c>
@@ -1762,15 +1693,15 @@
         <v>4446</v>
       </c>
       <c r="G17">
-        <v>1.012355086267893E-2</v>
+        <v>0.01012355086267893</v>
       </c>
       <c r="H17">
         <v>1.838709677419355</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1">
         <v>11</v>
       </c>
@@ -1784,15 +1715,15 @@
         <v>3407</v>
       </c>
       <c r="G18">
-        <v>1.1150379135258459E-2</v>
+        <v>0.01115037913525846</v>
       </c>
       <c r="H18">
-        <v>1.7086258776328991</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+        <v>1.708625877632899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
       <c r="C19" s="1">
         <v>12</v>
       </c>
@@ -1806,15 +1737,15 @@
         <v>5672</v>
       </c>
       <c r="G19">
-        <v>1.346804218678699E-2</v>
+        <v>0.01346804218678699</v>
       </c>
       <c r="H19">
-        <v>1.7960734642178591</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2">
+        <v>1.796073464217859</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1">
         <v>2013</v>
       </c>
       <c r="C20" s="1">
@@ -1830,15 +1761,15 @@
         <v>7257</v>
       </c>
       <c r="G20">
-        <v>1.276092581102123E-2</v>
+        <v>0.01276092581102123</v>
       </c>
       <c r="H20">
         <v>1.664449541284404</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
       <c r="C21" s="1">
         <v>2</v>
       </c>
@@ -1852,15 +1783,15 @@
         <v>3915</v>
       </c>
       <c r="G21">
-        <v>1.062073068165501E-2</v>
+        <v>0.01062073068165501</v>
       </c>
       <c r="H21">
-        <v>1.8903911154031869</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+        <v>1.890391115403187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1">
         <v>3</v>
       </c>
@@ -1874,15 +1805,15 @@
         <v>6455</v>
       </c>
       <c r="G22">
-        <v>1.195412555112324E-2</v>
+        <v>0.01195412555112324</v>
       </c>
       <c r="H22">
-        <v>1.7714050493962681</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+        <v>1.771405049396268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
       <c r="C23" s="1">
         <v>4</v>
       </c>
@@ -1896,15 +1827,15 @@
         <v>7752</v>
       </c>
       <c r="G23">
-        <v>9.956637448123128E-3</v>
+        <v>0.009956637448123128</v>
       </c>
       <c r="H23">
         <v>1.811214953271028</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="1">
         <v>5</v>
       </c>
@@ -1918,15 +1849,15 @@
         <v>9790</v>
       </c>
       <c r="G24">
-        <v>1.320901131294595E-2</v>
+        <v>0.01320901131294595</v>
       </c>
       <c r="H24">
-        <v>1.8086089044891931</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+        <v>1.808608904489193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
       <c r="C25" s="1">
         <v>6</v>
       </c>
@@ -1940,17 +1871,17 @@
         <v>13017</v>
       </c>
       <c r="G25">
-        <v>1.4078380796268049E-2</v>
+        <v>0.01407838079626805</v>
       </c>
       <c r="H25">
-        <v>1.7562061521856449</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+        <v>1.756206152185645</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>2012</v>
       </c>
       <c r="C26" s="1">
@@ -1966,15 +1897,15 @@
         <v>8700</v>
       </c>
       <c r="G26">
-        <v>3.0771750978156091E-2</v>
+        <v>0.03077175097815609</v>
       </c>
       <c r="H26">
         <v>1.781326781326781</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
       <c r="C27" s="1">
         <v>8</v>
       </c>
@@ -1988,15 +1919,15 @@
         <v>5760</v>
       </c>
       <c r="G27">
-        <v>2.0677007322837691E-2</v>
+        <v>0.02067700732283769</v>
       </c>
       <c r="H27">
-        <v>1.7988757026858211</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+        <v>1.798875702685821</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="1">
         <v>9</v>
       </c>
@@ -2010,15 +1941,15 @@
         <v>7869</v>
       </c>
       <c r="G28">
-        <v>2.5881685412517071E-2</v>
+        <v>0.02588168541251707</v>
       </c>
       <c r="H28">
-        <v>1.7969856131536881</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+        <v>1.796985613153688</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="1">
         <v>10</v>
       </c>
@@ -2032,15 +1963,15 @@
         <v>4505</v>
       </c>
       <c r="G29">
-        <v>2.319154498263435E-2</v>
+        <v>0.02319154498263435</v>
       </c>
       <c r="H29">
-        <v>1.8136070853462161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+        <v>1.813607085346216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="1">
         <v>11</v>
       </c>
@@ -2054,15 +1985,15 @@
         <v>5947</v>
       </c>
       <c r="G30">
-        <v>2.3026006438311569E-2</v>
+        <v>0.02302600643831157</v>
       </c>
       <c r="H30">
         <v>1.868363179390512</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
       <c r="C31" s="1">
         <v>12</v>
       </c>
@@ -2076,15 +2007,15 @@
         <v>9133</v>
       </c>
       <c r="G31">
-        <v>2.1015747550267892E-2</v>
+        <v>0.02101574755026789</v>
       </c>
       <c r="H31">
         <v>1.770647537805351</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2">
+    <row r="32" spans="1:8">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1">
         <v>2013</v>
       </c>
       <c r="C32" s="1">
@@ -2100,15 +2031,15 @@
         <v>6165</v>
       </c>
       <c r="G32">
-        <v>2.0698537675955801E-2</v>
+        <v>0.0206985376759558</v>
       </c>
       <c r="H32">
         <v>1.809509832697388</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="1">
         <v>2</v>
       </c>
@@ -2122,15 +2053,15 @@
         <v>4696</v>
       </c>
       <c r="G33">
-        <v>2.2267864942982739E-2</v>
+        <v>0.02226786494298274</v>
       </c>
       <c r="H33">
         <v>1.959933222036728</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="1">
         <v>3</v>
       </c>
@@ -2144,15 +2075,15 @@
         <v>8265</v>
       </c>
       <c r="G34">
-        <v>2.284464519681266E-2</v>
+        <v>0.02284464519681266</v>
       </c>
       <c r="H34">
         <v>1.844454362865432</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
       <c r="C35" s="1">
         <v>4</v>
       </c>
@@ -2166,15 +2097,15 @@
         <v>12994</v>
       </c>
       <c r="G35">
-        <v>2.4131212843245702E-2</v>
+        <v>0.0241312128432457</v>
       </c>
       <c r="H35">
-        <v>1.7994737570973549</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+        <v>1.799473757097355</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
       <c r="C36" s="1">
         <v>5</v>
       </c>
@@ -2188,15 +2119,15 @@
         <v>8631</v>
       </c>
       <c r="G36">
-        <v>2.1005369497577819E-2</v>
+        <v>0.02100536949757782</v>
       </c>
       <c r="H36">
         <v>1.798125</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
       <c r="C37" s="1">
         <v>6</v>
       </c>
@@ -2210,10 +2141,10 @@
         <v>13728</v>
       </c>
       <c r="G37">
-        <v>2.5229902443943492E-2</v>
+        <v>0.02522990244394349</v>
       </c>
       <c r="H37">
-        <v>1.7699845281072719</v>
+        <v>1.769984528107272</v>
       </c>
     </row>
   </sheetData>
@@ -2233,30 +2164,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="1">
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>2013</v>
@@ -2265,9 +2196,9 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -2276,9 +2207,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>136720</v>
@@ -2290,10 +2221,10 @@
         <v>-28750</v>
       </c>
       <c r="E4">
-        <v>-0.21028379169104741</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>-0.2102837916910474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2307,10 +2238,10 @@
         <v>224195</v>
       </c>
       <c r="E5">
-        <v>0.19250171083056641</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.1925017108305664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2324,12 +2255,12 @@
         <v>6149</v>
       </c>
       <c r="E6">
-        <v>0.21659797809010531</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.2165979780901053</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>51629</v>
@@ -2341,29 +2272,29 @@
         <v>10262</v>
       </c>
       <c r="E7">
-        <v>0.19876426039628889</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.1987642603962889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8">
-        <v>2.43757937008807E-2</v>
+        <v>0.0243757937008807</v>
       </c>
       <c r="C8">
-        <v>2.486834279690733E-2</v>
+        <v>0.02486834279690733</v>
       </c>
       <c r="D8">
-        <v>4.9254909602663294E-4</v>
+        <v>0.0004925490960266329</v>
       </c>
       <c r="E8">
-        <v>2.0206484435780121E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.02020648443578012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>1.818626932966994</v>
@@ -2372,10 +2303,10 @@
         <v>1.791968266836528</v>
       </c>
       <c r="D9">
-        <v>-2.6658666130466191E-2</v>
+        <v>-0.02665866613046619</v>
       </c>
       <c r="E9">
-        <v>-1.4658677734951379E-2</v>
+        <v>-0.01465867773495138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>